<commit_message>
Add calibration data of sensor 2
</commit_message>
<xml_diff>
--- a/data/calibration_N1.xlsx
+++ b/data/calibration_N1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DATALOG1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -44,14 +44,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="DATALOG2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/olegkirichenko/Documents/Arduino/ph_calibrate/data/DATALOG2.CSV" decimal="," thousands=" " comma="1">
+    <textPr fileType="mac" sourceFile="/Users/olegkirichenko/Documents/Arduino/ph_calibrate/data/DATALOG2.CSV" decimal="," thousands=" " comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="2" name="DATALOG3" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/olegkirichenko/Documents/Arduino/ph_calibrate/data/DATALOG3.CSV" decimal="," thousands=" " comma="1">
+    <textPr fileType="mac" sourceFile="/Users/olegkirichenko/Documents/Arduino/ph_calibrate/data/DATALOG3.CSV" decimal="," thousands=" " comma="1">
       <textFields>
         <textField/>
       </textFields>
@@ -187,7 +187,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -494,11 +493,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1204279664"/>
-        <c:axId val="-1204277888"/>
+        <c:axId val="975036496"/>
+        <c:axId val="975038816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1204279664"/>
+        <c:axId val="975036496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1204277888"/>
+        <c:crossAx val="975038816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,7 +548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1204277888"/>
+        <c:axId val="975038816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="805.0"/>
@@ -601,7 +600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1204279664"/>
+        <c:crossAx val="975036496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -615,7 +614,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -697,7 +695,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1004,11 +1001,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1203744240"/>
-        <c:axId val="-1203743712"/>
+        <c:axId val="974956432"/>
+        <c:axId val="974958752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1203744240"/>
+        <c:axId val="974956432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1203743712"/>
+        <c:crossAx val="974958752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1059,7 +1056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1203743712"/>
+        <c:axId val="974958752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="685.0"/>
@@ -1110,7 +1107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1203744240"/>
+        <c:crossAx val="974956432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,7 +1121,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1206,7 +1202,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1513,11 +1508,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1367652704"/>
-        <c:axId val="-1367651168"/>
+        <c:axId val="976916912"/>
+        <c:axId val="976919232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1367652704"/>
+        <c:axId val="976916912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1555,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1367651168"/>
+        <c:crossAx val="976919232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1568,7 +1563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1367651168"/>
+        <c:axId val="976919232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="590.0"/>
@@ -1620,7 +1615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1367652704"/>
+        <c:crossAx val="976916912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1634,7 +1629,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1881,11 +1875,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1207526624"/>
-        <c:axId val="-1203337728"/>
+        <c:axId val="975052768"/>
+        <c:axId val="975055088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1207526624"/>
+        <c:axId val="975052768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -1943,12 +1937,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1203337728"/>
+        <c:crossAx val="975055088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1203337728"/>
+        <c:axId val="975055088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2004,7 +1998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1207526624"/>
+        <c:crossAx val="975052768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4715,7 +4709,7 @@
         <v>797.42</v>
       </c>
       <c r="C2">
-        <f>$B$19</f>
+        <f t="shared" ref="C2:C17" si="0">$B$19</f>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4727,7 +4721,7 @@
         <v>802.03</v>
       </c>
       <c r="C3">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4739,7 +4733,7 @@
         <v>803.09</v>
       </c>
       <c r="C4">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4751,7 +4745,7 @@
         <v>803.11</v>
       </c>
       <c r="C5">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4763,7 +4757,7 @@
         <v>803.24</v>
       </c>
       <c r="C6">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4775,7 +4769,7 @@
         <v>803.3</v>
       </c>
       <c r="C7">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4787,7 +4781,7 @@
         <v>803.57</v>
       </c>
       <c r="C8">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4799,7 +4793,7 @@
         <v>803.6</v>
       </c>
       <c r="C9">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4811,7 +4805,7 @@
         <v>804.04</v>
       </c>
       <c r="C10">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4823,7 +4817,7 @@
         <v>803.53</v>
       </c>
       <c r="C11">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4835,7 +4829,7 @@
         <v>803.53</v>
       </c>
       <c r="C12">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4847,7 +4841,7 @@
         <v>803.89</v>
       </c>
       <c r="C13">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4859,7 +4853,7 @@
         <v>804.2</v>
       </c>
       <c r="C14">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4871,7 +4865,7 @@
         <v>803.86</v>
       </c>
       <c r="C15">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4883,7 +4877,7 @@
         <v>803.82</v>
       </c>
       <c r="C16">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4895,7 +4889,7 @@
         <v>804.52</v>
       </c>
       <c r="C17">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>803.88777777777773</v>
       </c>
     </row>
@@ -4958,7 +4952,7 @@
         <v>689.33</v>
       </c>
       <c r="C2">
-        <f>$B$19</f>
+        <f t="shared" ref="C2:C17" si="0">$B$19</f>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -4970,7 +4964,7 @@
         <v>693.49</v>
       </c>
       <c r="C3">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -4982,7 +4976,7 @@
         <v>693.76</v>
       </c>
       <c r="C4">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -4994,7 +4988,7 @@
         <v>693.44</v>
       </c>
       <c r="C5">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5006,7 +5000,7 @@
         <v>693.49</v>
       </c>
       <c r="C6">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5018,7 +5012,7 @@
         <v>694.18</v>
       </c>
       <c r="C7">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5030,7 +5024,7 @@
         <v>693.88</v>
       </c>
       <c r="C8">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5042,7 +5036,7 @@
         <v>694.07</v>
       </c>
       <c r="C9">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5054,7 +5048,7 @@
         <v>693.66</v>
       </c>
       <c r="C10">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5066,7 +5060,7 @@
         <v>693.89</v>
       </c>
       <c r="C11">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5078,7 +5072,7 @@
         <v>693.69</v>
       </c>
       <c r="C12">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5090,7 +5084,7 @@
         <v>693.42</v>
       </c>
       <c r="C13">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5102,7 +5096,7 @@
         <v>693.79</v>
       </c>
       <c r="C14">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5114,7 +5108,7 @@
         <v>693.74</v>
       </c>
       <c r="C15">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5126,7 +5120,7 @@
         <v>693.55</v>
       </c>
       <c r="C16">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5138,7 +5132,7 @@
         <v>693.42</v>
       </c>
       <c r="C17">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>693.69222222222231</v>
       </c>
     </row>
@@ -5197,7 +5191,7 @@
         <v>585.08000000000004</v>
       </c>
       <c r="C2">
-        <f>$B$19</f>
+        <f t="shared" ref="C2:C17" si="0">$B$19</f>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5209,7 +5203,7 @@
         <v>585.86</v>
       </c>
       <c r="C3">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5221,7 +5215,7 @@
         <v>585.66</v>
       </c>
       <c r="C4">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5233,7 +5227,7 @@
         <v>586.73</v>
       </c>
       <c r="C5">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5245,7 +5239,7 @@
         <v>585.69000000000005</v>
       </c>
       <c r="C6">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5257,7 +5251,7 @@
         <v>586.74</v>
       </c>
       <c r="C7">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5269,7 +5263,7 @@
         <v>586.30999999999995</v>
       </c>
       <c r="C8">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5281,7 +5275,7 @@
         <v>586.14</v>
       </c>
       <c r="C9">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5293,7 +5287,7 @@
         <v>586</v>
       </c>
       <c r="C10">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5305,7 +5299,7 @@
         <v>586.1</v>
       </c>
       <c r="C11">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5317,7 +5311,7 @@
         <v>585.70000000000005</v>
       </c>
       <c r="C12">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5329,7 +5323,7 @@
         <v>585.89</v>
       </c>
       <c r="C13">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5341,7 +5335,7 @@
         <v>585.87</v>
       </c>
       <c r="C14">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5353,7 +5347,7 @@
         <v>585.75</v>
       </c>
       <c r="C15">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5365,7 +5359,7 @@
         <v>586.26</v>
       </c>
       <c r="C16">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>
@@ -5377,7 +5371,7 @@
         <v>585.70000000000005</v>
       </c>
       <c r="C17">
-        <f>$B$19</f>
+        <f t="shared" si="0"/>
         <v>585.93444444444435</v>
       </c>
     </row>

</xml_diff>